<commit_message>
updated times on session schedule because times for session 17-20 only allowed 15 minutes
</commit_message>
<xml_diff>
--- a/SessionSlots-15minbreak.xlsx
+++ b/SessionSlots-15minbreak.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brao\Documents\Conference\JSConference\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\jsfriendsconf\ConferenceDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140124CD-FFC8-4626-9913-04D805656B7E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8E85DB-F432-4B8E-955A-C12469471B1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{145A6E31-CE10-427A-A3A4-19DD5E48F6FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t>11.50 AM to 12.45 PM</t>
   </si>
@@ -171,30 +170,9 @@
     <t>Potential Location  - Improving</t>
   </si>
   <si>
-    <t xml:space="preserve">9.00AM </t>
-  </si>
-  <si>
-    <t>10.15AM</t>
-  </si>
-  <si>
     <t>8.00 AM to 8.50AM</t>
   </si>
   <si>
-    <t>11.30AM</t>
-  </si>
-  <si>
-    <t>12.30PM</t>
-  </si>
-  <si>
-    <t>1.30PM</t>
-  </si>
-  <si>
-    <t>2.45PM</t>
-  </si>
-  <si>
-    <t>3.00PM</t>
-  </si>
-  <si>
     <t>4.15PM</t>
   </si>
   <si>
@@ -202,12 +180,51 @@
   </si>
   <si>
     <t xml:space="preserve">Meet SMEs for OpenSpace </t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>10.05AM to 10.55AM</t>
+  </si>
+  <si>
+    <t>11.10AM to 12.00PM</t>
+  </si>
+  <si>
+    <t>12.00PM to 1.00PM</t>
+  </si>
+  <si>
+    <t>1.00PM to 1.50PM</t>
+  </si>
+  <si>
+    <t>2.05PM to 2.55PM</t>
+  </si>
+  <si>
+    <t>3.10PM to 4.00PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -389,14 +406,56 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -404,9 +463,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -416,45 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D625DCEA-4119-4A3A-88D6-B797307D8391}">
-  <dimension ref="B1:H45"/>
+  <dimension ref="B1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42:F43"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,257 +802,258 @@
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" customWidth="1"/>
     <col min="8" max="8" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="B3" s="23">
         <v>43678</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="10" t="s">
+      <c r="D15" s="17"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="16">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="10">
         <v>43679</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="18"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="12"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="2" t="s">
         <v>35</v>
@@ -1055,262 +1074,345 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="21"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="21"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="21"/>
+      <c r="J31" s="28">
+        <v>0.375</v>
+      </c>
+      <c r="K31" s="28">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="L31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="21"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="21"/>
+      <c r="J33" s="28">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="K33" s="28">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="L33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="21"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="21"/>
+      <c r="J35" s="28">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="K35" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="L35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" s="21"/>
+      <c r="J36" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="K36" s="28">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="L36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="21"/>
+      <c r="J37" s="28">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K37" s="28">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="L37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="21"/>
+      <c r="J38" s="28">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="K38" s="28">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="L38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="21"/>
+      <c r="J39" s="28">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="K39" s="28">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="21"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="21"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="25"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="6"/>
-      <c r="H30" s="25"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="25"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
+      <c r="D42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="21"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="21"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="6"/>
-      <c r="H32" s="25"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="25"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="25"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="25"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H36" s="25"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="25"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="25"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="25"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G40" s="6"/>
-      <c r="H40" s="25"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="25"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="25"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="25"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="25"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="7"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="26"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="21"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="9"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="C5:G6"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C21:G22"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:G45"/>
+    <mergeCell ref="B3:G4"/>
+    <mergeCell ref="C13:G14"/>
+    <mergeCell ref="C7:D12"/>
+    <mergeCell ref="C15:D20"/>
+    <mergeCell ref="F7:G12"/>
+    <mergeCell ref="F15:G20"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
     <mergeCell ref="B25:H26"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="C28:G29"/>
@@ -1327,45 +1429,26 @@
     <mergeCell ref="E32:E33"/>
     <mergeCell ref="F32:F33"/>
     <mergeCell ref="G32:G33"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:G45"/>
-    <mergeCell ref="B3:G4"/>
-    <mergeCell ref="C13:G14"/>
-    <mergeCell ref="C7:D12"/>
-    <mergeCell ref="C15:D20"/>
-    <mergeCell ref="F7:G12"/>
-    <mergeCell ref="F15:G20"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C21:G22"/>
+    <mergeCell ref="C5:G6"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>